<commit_message>
sector 1 baseline analysis done
</commit_message>
<xml_diff>
--- a/data/Baseline Data.xlsx
+++ b/data/Baseline Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yezon\rqye\ECMA31320-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A98DE5C-C486-4D77-BE7D-12C8E427404E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EE92DD-9356-4B80-B975-7A01B76C2536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2CCB92FE-2352-46E7-B0C6-5682DE5195A1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="16">
   <si>
     <t>Instrument</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>GVC BP</t>
+  </si>
+  <si>
+    <t>GVC FP</t>
+  </si>
+  <si>
+    <t>Sector 1</t>
   </si>
 </sst>
 </file>
@@ -429,43 +435,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B81C45B-DC91-452C-A32E-C2EB2242502D}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -631,10 +637,658 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>17.670000000000002</v>
+      </c>
+      <c r="C12">
+        <v>21.335000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.40760000000000002</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>19.141999999999999</v>
+      </c>
+      <c r="C13">
+        <v>20.914000000000001</v>
+      </c>
+      <c r="D13">
+        <v>0.36009999999999998</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>-9.0934000000000008</v>
+      </c>
+      <c r="C14">
+        <v>26.204000000000001</v>
+      </c>
+      <c r="D14">
+        <v>0.72860000000000003</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>-2.4239999999999999</v>
+      </c>
+      <c r="C15">
+        <v>31.088999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.93789999999999996</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>2.0903</v>
+      </c>
+      <c r="C16">
+        <v>1.6584000000000001</v>
+      </c>
+      <c r="D16">
+        <v>0.20749999999999999</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>4.0403000000000002</v>
+      </c>
+      <c r="C17">
+        <v>2.4171999999999998</v>
+      </c>
+      <c r="D17">
+        <v>9.4600000000000004E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>2.7730999999999999</v>
+      </c>
+      <c r="C18">
+        <v>1.6815</v>
+      </c>
+      <c r="D18">
+        <v>9.9099999999999994E-2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>-267.57</v>
+      </c>
+      <c r="C21">
+        <v>1264.8</v>
+      </c>
+      <c r="D21">
+        <v>0.83240000000000003</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>-63.106000000000002</v>
+      </c>
+      <c r="C22">
+        <v>67.707999999999998</v>
+      </c>
+      <c r="D22">
+        <v>0.3513</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>88.198999999999998</v>
+      </c>
+      <c r="C23">
+        <v>380.19</v>
+      </c>
+      <c r="D23">
+        <v>0.8165</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>8.6608000000000001</v>
+      </c>
+      <c r="C24">
+        <v>109.6</v>
+      </c>
+      <c r="D24">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>266.64999999999998</v>
+      </c>
+      <c r="C25">
+        <v>2905.1</v>
+      </c>
+      <c r="D25">
+        <v>0.92689999999999995</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>24.321000000000002</v>
+      </c>
+      <c r="C26">
+        <v>42.203000000000003</v>
+      </c>
+      <c r="D26">
+        <v>0.56440000000000001</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>66.721999999999994</v>
+      </c>
+      <c r="C27">
+        <v>552.02</v>
+      </c>
+      <c r="D27">
+        <v>0.90380000000000005</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sector 1 baseline regressions done
</commit_message>
<xml_diff>
--- a/data/Baseline Data.xlsx
+++ b/data/Baseline Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yezon\rqye\ECMA31320-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EE92DD-9356-4B80-B975-7A01B76C2536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCE7C48-D3DF-4D03-9EB1-7DB4CE9349B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2CCB92FE-2352-46E7-B0C6-5682DE5195A1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="17">
   <si>
     <t>Instrument</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Sector 1</t>
+  </si>
+  <si>
+    <t>Sector 2</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B81C45B-DC91-452C-A32E-C2EB2242502D}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,6 +988,15 @@
       <c r="A30" t="s">
         <v>7</v>
       </c>
+      <c r="B30">
+        <v>-8.5996000000000006</v>
+      </c>
+      <c r="C30">
+        <v>15.019</v>
+      </c>
+      <c r="D30">
+        <v>0.56689999999999996</v>
+      </c>
       <c r="E30" t="s">
         <v>10</v>
       </c>
@@ -999,6 +1011,15 @@
       <c r="A31" t="s">
         <v>7</v>
       </c>
+      <c r="B31">
+        <v>-3.9148999999999998</v>
+      </c>
+      <c r="C31">
+        <v>3.9420999999999999</v>
+      </c>
+      <c r="D31">
+        <v>0.32069999999999999</v>
+      </c>
       <c r="E31" t="s">
         <v>10</v>
       </c>
@@ -1013,6 +1034,15 @@
       <c r="A32" t="s">
         <v>7</v>
       </c>
+      <c r="B32">
+        <v>-3.3772000000000002</v>
+      </c>
+      <c r="C32">
+        <v>15.942</v>
+      </c>
+      <c r="D32">
+        <v>0.83220000000000005</v>
+      </c>
       <c r="E32" t="s">
         <v>10</v>
       </c>
@@ -1027,6 +1057,15 @@
       <c r="A33" t="s">
         <v>7</v>
       </c>
+      <c r="B33">
+        <v>0.15570000000000001</v>
+      </c>
+      <c r="C33">
+        <v>8.0385000000000009</v>
+      </c>
+      <c r="D33">
+        <v>0.98450000000000004</v>
+      </c>
       <c r="E33" t="s">
         <v>11</v>
       </c>
@@ -1041,6 +1080,15 @@
       <c r="A34" t="s">
         <v>8</v>
       </c>
+      <c r="B34">
+        <v>-0.55649999999999999</v>
+      </c>
+      <c r="C34">
+        <v>0.84360000000000002</v>
+      </c>
+      <c r="D34">
+        <v>0.50949999999999995</v>
+      </c>
       <c r="E34" t="s">
         <v>10</v>
       </c>
@@ -1055,6 +1103,15 @@
       <c r="A35" t="s">
         <v>8</v>
       </c>
+      <c r="B35">
+        <v>-0.3266</v>
+      </c>
+      <c r="C35">
+        <v>1.1733</v>
+      </c>
+      <c r="D35">
+        <v>0.78069999999999995</v>
+      </c>
       <c r="E35" t="s">
         <v>10</v>
       </c>
@@ -1068,6 +1125,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>8</v>
+      </c>
+      <c r="B36">
+        <v>0.12570000000000001</v>
+      </c>
+      <c r="C36">
+        <v>0.78559999999999997</v>
+      </c>
+      <c r="D36">
+        <v>0.87290000000000001</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1091,6 +1157,15 @@
       <c r="A39" t="s">
         <v>7</v>
       </c>
+      <c r="B39">
+        <v>13.49</v>
+      </c>
+      <c r="C39">
+        <v>14.153</v>
+      </c>
+      <c r="D39">
+        <v>0.34050000000000002</v>
+      </c>
       <c r="E39" t="s">
         <v>10</v>
       </c>
@@ -1105,6 +1180,15 @@
       <c r="A40" t="s">
         <v>7</v>
       </c>
+      <c r="B40">
+        <v>12.590999999999999</v>
+      </c>
+      <c r="C40">
+        <v>11.974</v>
+      </c>
+      <c r="D40">
+        <v>0.29299999999999998</v>
+      </c>
       <c r="E40" t="s">
         <v>10</v>
       </c>
@@ -1119,6 +1203,15 @@
       <c r="A41" t="s">
         <v>7</v>
       </c>
+      <c r="B41">
+        <v>-5.43</v>
+      </c>
+      <c r="C41">
+        <v>16.382999999999999</v>
+      </c>
+      <c r="D41">
+        <v>0.74029999999999996</v>
+      </c>
       <c r="E41" t="s">
         <v>10</v>
       </c>
@@ -1133,6 +1226,15 @@
       <c r="A42" t="s">
         <v>7</v>
       </c>
+      <c r="B42">
+        <v>-1.8375999999999999</v>
+      </c>
+      <c r="C42">
+        <v>24.154</v>
+      </c>
+      <c r="D42">
+        <v>0.93940000000000001</v>
+      </c>
       <c r="E42" t="s">
         <v>11</v>
       </c>
@@ -1147,6 +1249,15 @@
       <c r="A43" t="s">
         <v>8</v>
       </c>
+      <c r="B43">
+        <v>-1.3339000000000001</v>
+      </c>
+      <c r="C43">
+        <v>2.1318000000000001</v>
+      </c>
+      <c r="D43">
+        <v>0.53149999999999997</v>
+      </c>
       <c r="E43" t="s">
         <v>10</v>
       </c>
@@ -1161,6 +1272,15 @@
       <c r="A44" t="s">
         <v>8</v>
       </c>
+      <c r="B44">
+        <v>-0.92610000000000003</v>
+      </c>
+      <c r="C44">
+        <v>2.0249000000000001</v>
+      </c>
+      <c r="D44">
+        <v>0.64739999999999998</v>
+      </c>
       <c r="E44" t="s">
         <v>10</v>
       </c>
@@ -1174,6 +1294,15 @@
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>8</v>
+      </c>
+      <c r="B45">
+        <v>-1.6332</v>
+      </c>
+      <c r="C45">
+        <v>2.0299</v>
+      </c>
+      <c r="D45">
+        <v>0.42109999999999997</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -1197,6 +1326,15 @@
       <c r="A48" t="s">
         <v>7</v>
       </c>
+      <c r="B48">
+        <v>-129.26</v>
+      </c>
+      <c r="C48">
+        <v>480.01</v>
+      </c>
+      <c r="D48">
+        <v>0.78769999999999996</v>
+      </c>
       <c r="E48" t="s">
         <v>10</v>
       </c>
@@ -1211,6 +1349,15 @@
       <c r="A49" t="s">
         <v>7</v>
       </c>
+      <c r="B49">
+        <v>-47.481000000000002</v>
+      </c>
+      <c r="C49">
+        <v>48.655000000000001</v>
+      </c>
+      <c r="D49">
+        <v>0.3291</v>
+      </c>
       <c r="E49" t="s">
         <v>10</v>
       </c>
@@ -1225,6 +1372,15 @@
       <c r="A50" t="s">
         <v>7</v>
       </c>
+      <c r="B50">
+        <v>-24.559000000000001</v>
+      </c>
+      <c r="C50">
+        <v>72.963999999999999</v>
+      </c>
+      <c r="D50">
+        <v>0.73640000000000005</v>
+      </c>
       <c r="E50" t="s">
         <v>10</v>
       </c>
@@ -1239,6 +1395,15 @@
       <c r="A51" t="s">
         <v>7</v>
       </c>
+      <c r="B51">
+        <v>-6.0121000000000002</v>
+      </c>
+      <c r="C51">
+        <v>77.754000000000005</v>
+      </c>
+      <c r="D51">
+        <v>0.93840000000000001</v>
+      </c>
       <c r="E51" t="s">
         <v>11</v>
       </c>
@@ -1253,6 +1418,15 @@
       <c r="A52" t="s">
         <v>8</v>
       </c>
+      <c r="B52">
+        <v>-3.5746000000000002</v>
+      </c>
+      <c r="C52">
+        <v>7.5008999999999997</v>
+      </c>
+      <c r="D52">
+        <v>0.63370000000000004</v>
+      </c>
       <c r="E52" t="s">
         <v>10</v>
       </c>
@@ -1267,6 +1441,15 @@
       <c r="A53" t="s">
         <v>8</v>
       </c>
+      <c r="B53">
+        <v>-1.3873</v>
+      </c>
+      <c r="C53">
+        <v>8.4610000000000003</v>
+      </c>
+      <c r="D53">
+        <v>0.86980000000000002</v>
+      </c>
       <c r="E53" t="s">
         <v>10</v>
       </c>
@@ -1281,6 +1464,15 @@
       <c r="A54" t="s">
         <v>8</v>
       </c>
+      <c r="B54">
+        <v>-29.277000000000001</v>
+      </c>
+      <c r="C54">
+        <v>137.35</v>
+      </c>
+      <c r="D54">
+        <v>0.83120000000000005</v>
+      </c>
       <c r="E54" t="s">
         <v>10</v>
       </c>
@@ -1288,6 +1480,324 @@
         <v>11</v>
       </c>
       <c r="G54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" t="s">
+        <v>11</v>
+      </c>
+      <c r="G60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" t="s">
+        <v>10</v>
+      </c>
+      <c r="G70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" t="s">
+        <v>10</v>
+      </c>
+      <c r="G76" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" t="s">
+        <v>11</v>
+      </c>
+      <c r="F78" t="s">
+        <v>11</v>
+      </c>
+      <c r="G78" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" t="s">
+        <v>10</v>
+      </c>
+      <c r="G79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>